<commit_message>
Fixed problem with corner cases, when n=1 the incorrect answers will not display properly.
</commit_message>
<xml_diff>
--- a/artikel/artikel.xlsx
+++ b/artikel/artikel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/Deutsch/artikel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/artikel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4ABE86-1118-A946-8C82-A0A275D29FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9517F650-7F6C-3D4D-8D92-2B8B3E688042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>